<commit_message>
Did some more analysis framing debt by population and area
</commit_message>
<xml_diff>
--- a/subnational-debt-OECD.xlsx
+++ b/subnational-debt-OECD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">Country</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">GDP Growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower quartile for population density</t>
   </si>
   <si>
     <t xml:space="preserve">Australia</t>
@@ -255,13 +258,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
+      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -297,10 +303,13 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>214</v>
@@ -332,10 +341,14 @@
       <c r="K2" s="1" t="n">
         <v>2.8</v>
       </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">IF(G2&lt;52, "True","False")</f>
+        <v>True</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>54.3</v>
@@ -367,10 +380,14 @@
       <c r="K3" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">IF(G3&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>97.2</v>
@@ -402,10 +419,14 @@
       <c r="K4" s="1" t="n">
         <v>1.5</v>
       </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">IF(G4&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1017.8</v>
@@ -437,10 +458,14 @@
       <c r="K5" s="1" t="n">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="0" t="str">
+        <f aca="false">IF(G5&lt;52, "True","False")</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>13.8</v>
@@ -472,10 +497,14 @@
       <c r="K6" s="1" t="n">
         <v>4.5</v>
       </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">IF(G6&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>29.4</v>
@@ -507,10 +536,14 @@
       <c r="K7" s="1" t="n">
         <v>1.6</v>
       </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">IF(G7&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1.7</v>
@@ -542,10 +575,14 @@
       <c r="K8" s="1" t="n">
         <v>1.4</v>
       </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">IF(G8&lt;52, "True","False")</f>
+        <v>True</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>27.3</v>
@@ -577,10 +614,14 @@
       <c r="K9" s="1" t="n">
         <v>0.2</v>
       </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">IF(G9&lt;52, "True","False")</f>
+        <v>True</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>287.6</v>
@@ -612,10 +653,14 @@
       <c r="K10" s="1" t="n">
         <v>1.3</v>
       </c>
+      <c r="L10" s="0" t="str">
+        <f aca="false">IF(G10&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>1104.5</v>
@@ -647,10 +692,14 @@
       <c r="K11" s="1" t="n">
         <v>1.7</v>
       </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">IF(G11&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>3.3</v>
@@ -682,10 +731,14 @@
       <c r="K12" s="1" t="n">
         <v>-0.2</v>
       </c>
+      <c r="L12" s="0" t="str">
+        <f aca="false">IF(G12&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>1.7</v>
@@ -717,10 +770,14 @@
       <c r="K13" s="1" t="n">
         <v>3.1</v>
       </c>
+      <c r="L13" s="0" t="str">
+        <f aca="false">IF(G13&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>1.8</v>
@@ -752,10 +809,14 @@
       <c r="K14" s="1" t="n">
         <v>4.2</v>
       </c>
+      <c r="L14" s="0" t="str">
+        <f aca="false">IF(G14&lt;52, "True","False")</f>
+        <v>True</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>7.1</v>
@@ -787,10 +848,14 @@
       <c r="K15" s="1" t="n">
         <v>26.3</v>
       </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">IF(G15&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>7.1</v>
@@ -822,10 +887,14 @@
       <c r="K16" s="1" t="n">
         <v>2.5</v>
       </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">IF(G16&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>259.2</v>
@@ -857,10 +926,14 @@
       <c r="K17" s="1" t="n">
         <v>0.7</v>
       </c>
+      <c r="L17" s="0" t="str">
+        <f aca="false">IF(G17&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>1742.4</v>
@@ -892,10 +965,14 @@
       <c r="K18" s="1" t="n">
         <v>0.6</v>
       </c>
+      <c r="L18" s="0" t="str">
+        <f aca="false">IF(G18&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>63.6</v>
@@ -927,10 +1004,14 @@
       <c r="K19" s="1" t="n">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L19" s="0" t="str">
+        <f aca="false">IF(G19&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>1.4</v>
@@ -962,10 +1043,14 @@
       <c r="K20" s="1" t="n">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L20" s="0" t="str">
+        <f aca="false">IF(G20&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>94.6</v>
@@ -997,10 +1082,14 @@
       <c r="K21" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="L21" s="0" t="str">
+        <f aca="false">IF(G21&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>52.6</v>
@@ -1032,10 +1121,14 @@
       <c r="K22" s="1" t="n">
         <v>1.6</v>
       </c>
+      <c r="L22" s="0" t="str">
+        <f aca="false">IF(G22&lt;52, "True","False")</f>
+        <v>True</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>54.5</v>
@@ -1067,10 +1160,14 @@
       <c r="K23" s="1" t="n">
         <v>3.9</v>
       </c>
+      <c r="L23" s="0" t="str">
+        <f aca="false">IF(G23&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>23</v>
@@ -1102,10 +1199,14 @@
       <c r="K24" s="1" t="n">
         <v>1.6</v>
       </c>
+      <c r="L24" s="0" t="str">
+        <f aca="false">IF(G24&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>4.8</v>
@@ -1137,10 +1238,14 @@
       <c r="K25" s="1" t="n">
         <v>3.8</v>
       </c>
+      <c r="L25" s="0" t="str">
+        <f aca="false">IF(G25&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>2.3</v>
@@ -1172,10 +1277,14 @@
       <c r="K26" s="1" t="n">
         <v>2.3</v>
       </c>
+      <c r="L26" s="0" t="str">
+        <f aca="false">IF(G26&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>492.4</v>
@@ -1207,10 +1316,14 @@
       <c r="K27" s="1" t="n">
         <v>3.2</v>
       </c>
+      <c r="L27" s="0" t="str">
+        <f aca="false">IF(G27&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>66.4</v>
@@ -1242,10 +1355,14 @@
       <c r="K28" s="1" t="n">
         <v>4.1</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L28" s="0" t="str">
+        <f aca="false">IF(G28&lt;52, "True","False")</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>112</v>
@@ -1277,10 +1394,14 @@
       <c r="K29" s="1" t="n">
         <v>0.8</v>
       </c>
+      <c r="L29" s="0" t="str">
+        <f aca="false">IF(G29&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>47.1</v>
@@ -1312,10 +1433,14 @@
       <c r="K30" s="1" t="n">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L30" s="0" t="str">
+        <f aca="false">IF(G30&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>264.4</v>
@@ -1347,10 +1472,14 @@
       <c r="K31" s="1" t="n">
         <v>2.2</v>
       </c>
+      <c r="L31" s="0" t="str">
+        <f aca="false">IF(G31&lt;52, "True","False")</f>
+        <v>False</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>5126.8</v>
@@ -1381,6 +1510,10 @@
       </c>
       <c r="K32" s="1" t="n">
         <v>2.6</v>
+      </c>
+      <c r="L32" s="0" t="str">
+        <f aca="false">IF(G32&lt;52, "True","False")</f>
+        <v>True</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>